<commit_message>
added benchmarking code for matrix sizes and major rename of dest to origin constrained which was a mistake
</commit_message>
<xml_diff>
--- a/results/TFModelRunTimes.xlsx
+++ b/results/TFModelRunTimes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>secs</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>1 run</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>CPU</t>
   </si>
 </sst>
 </file>
@@ -611,7 +617,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>MatrixResizeRuns1000!$D$1</c:f>
+              <c:f>MatrixResizeRuns1000!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -634,7 +640,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>MatrixResizeRuns1000!$A$2:$A$47</c:f>
+              <c:f>MatrixResizeRuns1000!$A$3:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
@@ -781,7 +787,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MatrixResizeRuns1000!$D$2:$D$47</c:f>
+              <c:f>MatrixResizeRuns1000!$D$3:$D$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
@@ -930,6 +936,255 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2077-43AE-8E79-AEA17D23A429}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MatrixResizeRuns1000!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MatrixResizeRuns1000!$F$3:$F$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7201</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MatrixResizeRuns1000!$I$3:$I$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>1.1403207778930599E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4236440658569301E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9397516250610299E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3497974872589102E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.03900876045227E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.38890583515167E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7995713233947701E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2606072187423699E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8165900468826201E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3519831657409599E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0399931669235202E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.6794223308563199E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.38542137145996E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.1526825428008997E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.0246840000152508E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.8833922147750798E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.8392498493194499E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.8372735500335692E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.107749403715133</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.121980296134948</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.18118343520164398</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25564385557174601</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.33940468215942299</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.43449460196494999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.54282770919799805</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.66999098062515205</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.80698029637336699</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.953758783578872</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1185817229747699</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.30666471123695</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.39509564375877</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.4907091047763799</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.66696703839302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1CC-4847-9B89-F646052C9647}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2388,13 +2643,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2998,10 +3253,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3009,707 +3264,1174 @@
     <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>100</v>
       </c>
-      <c r="B2">
-        <v>1000</v>
-      </c>
-      <c r="C2">
+      <c r="B3">
+        <v>1000</v>
+      </c>
+      <c r="C3">
         <v>1.2372918128967201</v>
       </c>
-      <c r="D2">
-        <f>C2/B2</f>
+      <c r="D3">
+        <f t="shared" ref="D3:D48" si="0">C3/B3</f>
         <v>1.2372918128967202E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
+        <v>1.14032077789306</v>
+      </c>
+      <c r="I3">
+        <f>H3/G3</f>
+        <v>1.1403207778930599E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>200</v>
       </c>
-      <c r="B3">
-        <v>1000</v>
-      </c>
-      <c r="C3">
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
         <v>1.78695440292358</v>
       </c>
-      <c r="D3">
-        <f>C3/B3</f>
+      <c r="D4">
+        <f t="shared" si="0"/>
         <v>1.78695440292358E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F4">
+        <v>200</v>
+      </c>
+      <c r="G4">
+        <v>1000</v>
+      </c>
+      <c r="H4">
+        <v>2.42364406585693</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I35" si="1">H4/G4</f>
+        <v>2.4236440658569301E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>300</v>
       </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5">
         <v>1.5421159267425499</v>
       </c>
-      <c r="D4">
-        <f>C4/B4</f>
+      <c r="D5">
+        <f t="shared" si="0"/>
         <v>1.54211592674255E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F5">
+        <v>300</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5">
+        <v>3.9397516250610298</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>3.9397516250610299E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>400</v>
       </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5">
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
         <v>2.1787550449371298</v>
       </c>
-      <c r="D5">
-        <f>C5/B5</f>
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>2.1787550449371296E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F6">
+        <v>400</v>
+      </c>
+      <c r="G6">
+        <v>1000</v>
+      </c>
+      <c r="H6">
+        <v>7.3497974872589102</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>7.3497974872589102E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>500</v>
       </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6">
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7">
         <v>2.3836107254028298</v>
       </c>
-      <c r="D6">
-        <f>C6/B6</f>
+      <c r="D7">
+        <f t="shared" si="0"/>
         <v>2.3836107254028298E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F7">
+        <v>500</v>
+      </c>
+      <c r="G7">
+        <v>1000</v>
+      </c>
+      <c r="H7">
+        <v>10.3900876045227</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1.03900876045227E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>600</v>
       </c>
-      <c r="B7">
-        <v>1000</v>
-      </c>
-      <c r="C7">
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8">
         <v>3.6928846836089999</v>
       </c>
-      <c r="D7">
-        <f>C7/B7</f>
+      <c r="D8">
+        <f t="shared" si="0"/>
         <v>3.6928846836089997E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F8">
+        <v>600</v>
+      </c>
+      <c r="G8">
+        <v>1000</v>
+      </c>
+      <c r="H8">
+        <v>13.889058351516701</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1.38890583515167E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>700</v>
       </c>
-      <c r="B8">
-        <v>1000</v>
-      </c>
-      <c r="C8">
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
         <v>4.80722880363464</v>
       </c>
-      <c r="D8">
-        <f>C8/B8</f>
+      <c r="D9">
+        <f t="shared" si="0"/>
         <v>4.8072288036346399E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="F9">
+        <v>700</v>
+      </c>
+      <c r="G9">
+        <v>1000</v>
+      </c>
+      <c r="H9">
+        <v>17.995713233947701</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1.7995713233947701E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>800</v>
       </c>
-      <c r="B9">
-        <v>1000</v>
-      </c>
-      <c r="C9">
+      <c r="B10">
+        <v>1000</v>
+      </c>
+      <c r="C10">
         <v>6.2703883647918701</v>
       </c>
-      <c r="D9">
-        <f>C9/B9</f>
+      <c r="D10">
+        <f t="shared" si="0"/>
         <v>6.2703883647918703E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="F10">
+        <v>800</v>
+      </c>
+      <c r="G10">
+        <v>1000</v>
+      </c>
+      <c r="H10">
+        <v>22.606072187423699</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>2.2606072187423699E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>900</v>
       </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-      <c r="C10">
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11">
         <v>7.3768093585968</v>
       </c>
-      <c r="D10">
-        <f>C10/B10</f>
+      <c r="D11">
+        <f t="shared" si="0"/>
         <v>7.3768093585967996E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1000</v>
-      </c>
-      <c r="B11">
-        <v>1000</v>
-      </c>
-      <c r="C11">
+      <c r="F11">
+        <v>900</v>
+      </c>
+      <c r="G11">
+        <v>1000</v>
+      </c>
+      <c r="H11">
+        <v>28.165900468826202</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>2.8165900468826201E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12">
         <v>8.4911649227142298</v>
       </c>
-      <c r="D11">
-        <f>C11/B11</f>
+      <c r="D12">
+        <f t="shared" si="0"/>
         <v>8.4911649227142304E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="F12">
+        <v>1000</v>
+      </c>
+      <c r="G12">
+        <v>1000</v>
+      </c>
+      <c r="H12">
+        <v>33.519831657409597</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>3.3519831657409599E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>1100</v>
       </c>
-      <c r="B12">
-        <v>1000</v>
-      </c>
-      <c r="C12">
+      <c r="B13">
+        <v>1000</v>
+      </c>
+      <c r="C13">
         <v>10.678885936737</v>
       </c>
-      <c r="D12">
-        <f>C12/B12</f>
+      <c r="D13">
+        <f t="shared" si="0"/>
         <v>1.0678885936737E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="F13">
+        <v>1100</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+      <c r="H13">
+        <v>40.399931669235201</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>4.0399931669235202E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>1200</v>
       </c>
-      <c r="B13">
-        <v>1000</v>
-      </c>
-      <c r="C13">
+      <c r="B14">
+        <v>1000</v>
+      </c>
+      <c r="C14">
         <v>12.0431332588195</v>
       </c>
-      <c r="D13">
-        <f>C13/B13</f>
+      <c r="D14">
+        <f t="shared" si="0"/>
         <v>1.20431332588195E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="F14">
+        <v>1200</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="H14">
+        <v>46.794223308563197</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>4.6794223308563199E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>1300</v>
       </c>
-      <c r="B14">
-        <v>1000</v>
-      </c>
-      <c r="C14">
+      <c r="B15">
+        <v>1000</v>
+      </c>
+      <c r="C15">
         <v>14.239826917648299</v>
       </c>
-      <c r="D14">
-        <f>C14/B14</f>
+      <c r="D15">
+        <f t="shared" si="0"/>
         <v>1.42398269176483E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="F15">
+        <v>1300</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+      <c r="H15">
+        <v>53.854213714599602</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>5.38542137145996E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>1400</v>
       </c>
-      <c r="B15">
-        <v>1000</v>
-      </c>
-      <c r="C15">
+      <c r="B16">
+        <v>1000</v>
+      </c>
+      <c r="C16">
         <v>15.379177331924399</v>
       </c>
-      <c r="D15">
-        <f>C15/B15</f>
+      <c r="D16">
+        <f t="shared" si="0"/>
         <v>1.53791773319244E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="F16">
+        <v>1400</v>
+      </c>
+      <c r="G16">
+        <v>1000</v>
+      </c>
+      <c r="H16">
+        <v>61.526825428008998</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>6.1526825428008997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>1500</v>
       </c>
-      <c r="B16">
-        <v>1000</v>
-      </c>
-      <c r="C16">
+      <c r="B17">
+        <v>1000</v>
+      </c>
+      <c r="C17">
         <v>19.0081112384796</v>
       </c>
-      <c r="D16">
-        <f>C16/B16</f>
+      <c r="D17">
+        <f t="shared" si="0"/>
         <v>1.9008111238479598E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="F17">
+        <v>1500</v>
+      </c>
+      <c r="G17">
+        <v>1000</v>
+      </c>
+      <c r="H17">
+        <v>70.246840000152503</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>7.0246840000152508E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>1600</v>
       </c>
-      <c r="B17">
-        <v>1000</v>
-      </c>
-      <c r="C17">
+      <c r="B18">
+        <v>1000</v>
+      </c>
+      <c r="C18">
         <v>21.1129937171936</v>
       </c>
-      <c r="D17">
-        <f>C17/B17</f>
+      <c r="D18">
+        <f t="shared" si="0"/>
         <v>2.11129937171936E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="F18">
+        <v>1600</v>
+      </c>
+      <c r="G18">
+        <v>1000</v>
+      </c>
+      <c r="H18">
+        <v>78.833922147750798</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>7.8833922147750798E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>1700</v>
       </c>
-      <c r="B18">
-        <v>1000</v>
-      </c>
-      <c r="C18">
+      <c r="B19">
+        <v>1000</v>
+      </c>
+      <c r="C19">
         <v>23.6794543266296</v>
       </c>
-      <c r="D18">
-        <f>C18/B18</f>
+      <c r="D19">
+        <f t="shared" si="0"/>
         <v>2.3679454326629601E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="F19">
+        <v>1700</v>
+      </c>
+      <c r="G19">
+        <v>1000</v>
+      </c>
+      <c r="H19">
+        <v>88.392498493194495</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>8.8392498493194499E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>1800</v>
       </c>
-      <c r="B19">
-        <v>1000</v>
-      </c>
-      <c r="C19">
+      <c r="B20">
+        <v>1000</v>
+      </c>
+      <c r="C20">
         <v>25.052642345428399</v>
       </c>
-      <c r="D19">
-        <f>C19/B19</f>
+      <c r="D20">
+        <f t="shared" si="0"/>
         <v>2.5052642345428398E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="F20">
+        <v>1800</v>
+      </c>
+      <c r="G20">
+        <v>1000</v>
+      </c>
+      <c r="H20">
+        <v>98.372735500335693</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>9.8372735500335692E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>1900</v>
       </c>
-      <c r="B20">
-        <v>1000</v>
-      </c>
-      <c r="C20">
+      <c r="B21">
+        <v>1000</v>
+      </c>
+      <c r="C21">
         <v>26.848642826080301</v>
       </c>
-      <c r="D20">
-        <f>C20/B20</f>
+      <c r="D21">
+        <f t="shared" si="0"/>
         <v>2.68486428260803E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="F21">
+        <v>1900</v>
+      </c>
+      <c r="G21">
+        <v>1000</v>
+      </c>
+      <c r="H21">
+        <v>107.749403715133</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0.107749403715133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>2000</v>
       </c>
-      <c r="B21">
-        <v>1000</v>
-      </c>
-      <c r="C21">
+      <c r="B22">
+        <v>1000</v>
+      </c>
+      <c r="C22">
         <v>28.970450162887499</v>
       </c>
-      <c r="D21">
-        <f>C21/B21</f>
+      <c r="D22">
+        <f t="shared" si="0"/>
         <v>2.8970450162887497E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="F22">
+        <v>2000</v>
+      </c>
+      <c r="G22">
+        <v>1000</v>
+      </c>
+      <c r="H22">
+        <v>121.98029613494801</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0.121980296134948</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>2500</v>
       </c>
-      <c r="B22">
-        <v>1000</v>
-      </c>
-      <c r="C22">
+      <c r="B23">
+        <v>1000</v>
+      </c>
+      <c r="C23">
         <v>44.467584371566701</v>
       </c>
-      <c r="D22">
-        <f>C22/B22</f>
+      <c r="D23">
+        <f t="shared" si="0"/>
         <v>4.4467584371566699E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="F23">
+        <v>2500</v>
+      </c>
+      <c r="G23">
+        <v>1000</v>
+      </c>
+      <c r="H23">
+        <v>181.18343520164399</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0.18118343520164398</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>3000</v>
       </c>
-      <c r="B23">
-        <v>1000</v>
-      </c>
-      <c r="C23">
+      <c r="B24">
+        <v>1000</v>
+      </c>
+      <c r="C24">
         <v>59.182149648666297</v>
       </c>
-      <c r="D23">
-        <f>C23/B23</f>
+      <c r="D24">
+        <f t="shared" si="0"/>
         <v>5.9182149648666298E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="F24">
+        <v>3000</v>
+      </c>
+      <c r="G24">
+        <v>1000</v>
+      </c>
+      <c r="H24">
+        <v>255.643855571746</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>0.25564385557174601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>3500</v>
       </c>
-      <c r="B24">
-        <v>1000</v>
-      </c>
-      <c r="C24">
+      <c r="B25">
+        <v>1000</v>
+      </c>
+      <c r="C25">
         <v>78.739933252334595</v>
       </c>
-      <c r="D24">
-        <f>C24/B24</f>
+      <c r="D25">
+        <f t="shared" si="0"/>
         <v>7.8739933252334596E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="F25">
+        <v>3500</v>
+      </c>
+      <c r="G25">
+        <v>1000</v>
+      </c>
+      <c r="H25">
+        <v>339.40468215942298</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>0.33940468215942299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>4000</v>
       </c>
-      <c r="B25">
-        <v>1000</v>
-      </c>
-      <c r="C25">
+      <c r="B26">
+        <v>1000</v>
+      </c>
+      <c r="C26">
         <v>100.770351886749</v>
       </c>
-      <c r="D25">
-        <f>C25/B25</f>
+      <c r="D26">
+        <f t="shared" si="0"/>
         <v>0.100770351886749</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="F26">
+        <v>4000</v>
+      </c>
+      <c r="G26">
+        <v>1000</v>
+      </c>
+      <c r="H26">
+        <v>434.49460196494999</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0.43449460196494999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>4500</v>
       </c>
-      <c r="B26">
-        <v>1000</v>
-      </c>
-      <c r="C26">
+      <c r="B27">
+        <v>1000</v>
+      </c>
+      <c r="C27">
         <v>122.412969350814</v>
       </c>
-      <c r="D26">
-        <f>C26/B26</f>
+      <c r="D27">
+        <f t="shared" si="0"/>
         <v>0.122412969350814</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="F27">
+        <v>4500</v>
+      </c>
+      <c r="G27">
+        <v>1000</v>
+      </c>
+      <c r="H27">
+        <v>542.82770919799805</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>0.54282770919799805</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>5000</v>
       </c>
-      <c r="B27">
-        <v>1000</v>
-      </c>
-      <c r="C27">
+      <c r="B28">
+        <v>1000</v>
+      </c>
+      <c r="C28">
         <v>147.816450595855</v>
       </c>
-      <c r="D27">
-        <f>C27/B27</f>
+      <c r="D28">
+        <f t="shared" si="0"/>
         <v>0.14781645059585499</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="F28">
+        <v>5000</v>
+      </c>
+      <c r="G28">
+        <v>1000</v>
+      </c>
+      <c r="H28">
+        <v>669.99098062515202</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>0.66999098062515205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>5500</v>
       </c>
-      <c r="B28">
-        <v>1000</v>
-      </c>
-      <c r="C28">
+      <c r="B29">
+        <v>1000</v>
+      </c>
+      <c r="C29">
         <v>177.505316019058</v>
       </c>
-      <c r="D28">
-        <f>C28/B28</f>
+      <c r="D29">
+        <f t="shared" si="0"/>
         <v>0.177505316019058</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="F29">
+        <v>5500</v>
+      </c>
+      <c r="G29">
+        <v>1000</v>
+      </c>
+      <c r="H29">
+        <v>806.98029637336697</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0.80698029637336699</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>6000</v>
       </c>
-      <c r="B29">
-        <v>1000</v>
-      </c>
-      <c r="C29">
+      <c r="B30">
+        <v>1000</v>
+      </c>
+      <c r="C30">
         <v>208.72721719741801</v>
       </c>
-      <c r="D29">
-        <f>C29/B29</f>
+      <c r="D30">
+        <f t="shared" si="0"/>
         <v>0.20872721719741802</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="F30">
+        <v>6000</v>
+      </c>
+      <c r="G30">
+        <v>1000</v>
+      </c>
+      <c r="H30">
+        <v>953.758783578872</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>0.953758783578872</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>6500</v>
       </c>
-      <c r="B30">
-        <v>1000</v>
-      </c>
-      <c r="C30">
+      <c r="B31">
+        <v>1000</v>
+      </c>
+      <c r="C31">
         <v>243.53566646575899</v>
       </c>
-      <c r="D30">
-        <f>C30/B30</f>
+      <c r="D31">
+        <f t="shared" si="0"/>
         <v>0.243535666465759</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="F31">
+        <v>6500</v>
+      </c>
+      <c r="G31">
+        <v>1000</v>
+      </c>
+      <c r="H31">
+        <v>1118.5817229747699</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>1.1185817229747699</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>7000</v>
       </c>
-      <c r="B31">
-        <v>1000</v>
-      </c>
-      <c r="C31">
+      <c r="B32">
+        <v>1000</v>
+      </c>
+      <c r="C32">
         <v>276.35051941871598</v>
       </c>
-      <c r="D31">
-        <f>C31/B31</f>
+      <c r="D32">
+        <f t="shared" si="0"/>
         <v>0.27635051941871597</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="F32">
+        <v>7000</v>
+      </c>
+      <c r="G32">
+        <v>1000</v>
+      </c>
+      <c r="H32">
+        <v>1306.6647112369501</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>1.30666471123695</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>7201</v>
       </c>
-      <c r="B32">
-        <v>1000</v>
-      </c>
-      <c r="C32">
+      <c r="B33">
+        <v>1000</v>
+      </c>
+      <c r="C33">
         <v>297.70272850990199</v>
       </c>
-      <c r="D32">
-        <f>C32/B32</f>
+      <c r="D33">
+        <f t="shared" si="0"/>
         <v>0.29770272850990198</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="F33">
+        <v>7201</v>
+      </c>
+      <c r="G33">
+        <v>1000</v>
+      </c>
+      <c r="H33">
+        <v>1395.0956437587699</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>1.39509564375877</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>7500</v>
       </c>
-      <c r="B33">
-        <v>1000</v>
-      </c>
-      <c r="C33">
+      <c r="B34">
+        <v>1000</v>
+      </c>
+      <c r="C34">
         <v>316.38594770431502</v>
       </c>
-      <c r="D33">
-        <f>C33/B33</f>
+      <c r="D34">
+        <f t="shared" si="0"/>
         <v>0.316385947704315</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="F34">
+        <v>7500</v>
+      </c>
+      <c r="G34">
+        <v>1000</v>
+      </c>
+      <c r="H34">
+        <v>1490.7091047763799</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>1.4907091047763799</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>8000</v>
       </c>
-      <c r="B34">
-        <v>1000</v>
-      </c>
-      <c r="C34">
+      <c r="B35">
+        <v>1000</v>
+      </c>
+      <c r="C35">
         <v>355.09769439697197</v>
       </c>
-      <c r="D34">
-        <f>C34/B34</f>
+      <c r="D35">
+        <f t="shared" si="0"/>
         <v>0.35509769439697197</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="F35">
+        <v>8000</v>
+      </c>
+      <c r="G35">
+        <v>1000</v>
+      </c>
+      <c r="H35">
+        <v>1666.9670383930199</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>1.66696703839302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>8500</v>
       </c>
-      <c r="B35">
-        <v>1000</v>
-      </c>
-      <c r="C35">
+      <c r="B36">
+        <v>1000</v>
+      </c>
+      <c r="C36">
         <v>393.90226984024002</v>
       </c>
-      <c r="D35">
-        <f>C35/B35</f>
+      <c r="D36">
+        <f t="shared" si="0"/>
         <v>0.39390226984024002</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>9000</v>
       </c>
-      <c r="B36">
-        <v>1000</v>
-      </c>
-      <c r="C36">
+      <c r="B37">
+        <v>1000</v>
+      </c>
+      <c r="C37">
         <v>409.89277434348998</v>
       </c>
-      <c r="D36">
-        <f>C36/B36</f>
+      <c r="D37">
+        <f t="shared" si="0"/>
         <v>0.40989277434348997</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>9500</v>
       </c>
-      <c r="B37">
-        <v>1000</v>
-      </c>
-      <c r="C37">
+      <c r="B38">
+        <v>1000</v>
+      </c>
+      <c r="C38">
         <v>479.55365467071499</v>
       </c>
-      <c r="D37">
-        <f>C37/B37</f>
+      <c r="D38">
+        <f t="shared" si="0"/>
         <v>0.47955365467071498</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>10000</v>
       </c>
-      <c r="B38">
-        <v>1000</v>
-      </c>
-      <c r="C38">
+      <c r="B39">
+        <v>1000</v>
+      </c>
+      <c r="C39">
         <v>529.32760858535698</v>
       </c>
-      <c r="D38">
-        <f>C38/B38</f>
+      <c r="D39">
+        <f t="shared" si="0"/>
         <v>0.52932760858535699</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>10500</v>
       </c>
-      <c r="B39">
-        <v>1000</v>
-      </c>
-      <c r="C39">
+      <c r="B40">
+        <v>1000</v>
+      </c>
+      <c r="C40">
         <v>545.56209588050797</v>
       </c>
-      <c r="D39">
-        <f>C39/B39</f>
+      <c r="D40">
+        <f t="shared" si="0"/>
         <v>0.54556209588050797</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>11000</v>
       </c>
-      <c r="B40">
-        <v>1000</v>
-      </c>
-      <c r="C40">
+      <c r="B41">
+        <v>1000</v>
+      </c>
+      <c r="C41">
         <v>548.75197768211297</v>
       </c>
-      <c r="D40">
-        <f>C40/B40</f>
+      <c r="D41">
+        <f t="shared" si="0"/>
         <v>0.54875197768211292</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>11500</v>
       </c>
-      <c r="B41">
-        <v>1000</v>
-      </c>
-      <c r="C41">
+      <c r="B42">
+        <v>1000</v>
+      </c>
+      <c r="C42">
         <v>602.04014563560395</v>
       </c>
-      <c r="D41">
-        <f>C41/B41</f>
+      <c r="D42">
+        <f t="shared" si="0"/>
         <v>0.60204014563560393</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>12000</v>
       </c>
-      <c r="B42">
-        <v>1000</v>
-      </c>
-      <c r="C42">
+      <c r="B43">
+        <v>1000</v>
+      </c>
+      <c r="C43">
         <v>655.29167199134804</v>
       </c>
-      <c r="D42">
-        <f>C42/B42</f>
+      <c r="D43">
+        <f t="shared" si="0"/>
         <v>0.65529167199134808</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>12500</v>
       </c>
-      <c r="B43">
-        <v>1000</v>
-      </c>
-      <c r="C43">
+      <c r="B44">
+        <v>1000</v>
+      </c>
+      <c r="C44">
         <v>709.62730574607804</v>
       </c>
-      <c r="D43">
-        <f>C43/B43</f>
+      <c r="D44">
+        <f t="shared" si="0"/>
         <v>0.70962730574607802</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>13000</v>
       </c>
-      <c r="B44">
-        <v>1000</v>
-      </c>
-      <c r="C44">
+      <c r="B45">
+        <v>1000</v>
+      </c>
+      <c r="C45">
         <v>767.81599926948502</v>
       </c>
-      <c r="D44">
-        <f>C44/B44</f>
+      <c r="D45">
+        <f t="shared" si="0"/>
         <v>0.76781599926948507</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>14000</v>
       </c>
-      <c r="B45">
-        <v>1000</v>
-      </c>
-      <c r="C45">
+      <c r="B46">
+        <v>1000</v>
+      </c>
+      <c r="C46">
         <v>888.65862679481495</v>
       </c>
-      <c r="D45">
-        <f>C45/B45</f>
+      <c r="D46">
+        <f t="shared" si="0"/>
         <v>0.888658626794815</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>15000</v>
       </c>
-      <c r="B46">
-        <v>1000</v>
-      </c>
-      <c r="C46">
+      <c r="B47">
+        <v>1000</v>
+      </c>
+      <c r="C47">
         <v>1007.79523706436</v>
       </c>
-      <c r="D46">
-        <f>C46/B46</f>
+      <c r="D47">
+        <f t="shared" si="0"/>
         <v>1.0077952370643599</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>16000</v>
       </c>
-      <c r="B47">
-        <v>1000</v>
-      </c>
-      <c r="C47">
+      <c r="B48">
+        <v>1000</v>
+      </c>
+      <c r="C48">
         <v>1157.3927581310199</v>
       </c>
-      <c r="D47">
-        <f>C47/B47</f>
+      <c r="D48">
+        <f t="shared" si="0"/>
         <v>1.1573927581310199</v>
       </c>
     </row>

</xml_diff>